<commit_message>
Finished up the Report
Finished the normalization report.
</commit_message>
<xml_diff>
--- a/Phase 3 Normalization.xlsx
+++ b/Phase 3 Normalization.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connar\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connar\Documents\GitHub\PROG2111-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF889BE-65C4-40E7-BE5D-F45BA2DEABC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AE50E2-4213-4FB2-9E43-1EB3C6F3125B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{ED13D5FD-5B9F-4291-912E-FF72C27A7752}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="88">
   <si>
     <t>1st Form</t>
   </si>
@@ -294,6 +294,12 @@
   </si>
   <si>
     <t>null</t>
+  </si>
+  <si>
+    <t>Payment Table</t>
+  </si>
+  <si>
+    <t>Quantity</t>
   </si>
 </sst>
 </file>
@@ -418,7 +424,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -433,11 +439,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -773,10 +777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893056DF-6DF6-445A-A96E-94814F31D4EC}">
-  <dimension ref="A1:Z62"/>
+  <dimension ref="A1:AA62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -807,12 +811,12 @@
     <col min="25" max="25" width="12.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -888,11 +892,14 @@
       <c r="Y2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="Z2" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AA2" s="14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>1001</v>
       </c>
@@ -968,11 +975,14 @@
       <c r="Y3" s="5">
         <v>45820</v>
       </c>
-      <c r="Z3" s="6">
+      <c r="Z3" s="13">
         <v>19.989999999999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AA3" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>1002</v>
       </c>
@@ -1048,11 +1058,14 @@
       <c r="Y4" s="5">
         <v>45836</v>
       </c>
-      <c r="Z4" s="6">
+      <c r="Z4" s="13">
         <v>119.98</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA4" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>1002</v>
       </c>
@@ -1128,11 +1141,14 @@
       <c r="Y5" s="5">
         <v>45836</v>
       </c>
-      <c r="Z5" s="6">
+      <c r="Z5" s="13">
         <v>119.98</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA5" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <v>1003</v>
       </c>
@@ -1208,17 +1224,25 @@
       <c r="Y6" s="9">
         <v>45841</v>
       </c>
-      <c r="Z6" s="10">
+      <c r="Z6" s="8">
         <v>79.989999999999995</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" ht="11.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA6" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="11.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -1240,89 +1264,101 @@
       <c r="G10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="I10" s="14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>1001</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11">
         <v>10</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="5">
         <v>45820</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="13">
         <v>19.989999999999998</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="I11" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>1002</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12">
         <v>12</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="5">
         <v>45836</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="13">
         <v>119.98</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="I12" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>1002</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13">
         <v>3</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="5">
         <v>45836</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="13">
         <v>119.98</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="I13" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A14" s="7">
         <v>1003</v>
       </c>
@@ -1344,8 +1380,16 @@
       <c r="G14" s="9">
         <v>45841</v>
       </c>
-      <c r="H14" s="10">
+      <c r="H14" s="8">
         <v>79.989999999999995</v>
+      </c>
+      <c r="I14" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -1408,6 +1452,11 @@
         <v>98765432</v>
       </c>
     </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>40</v>
@@ -1435,19 +1484,19 @@
       <c r="A23" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" t="s">
         <v>62</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" t="s">
         <v>63</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="14">
+      <c r="F23" s="5">
         <v>45790</v>
       </c>
       <c r="G23" s="6">
@@ -1458,19 +1507,19 @@
       <c r="A24" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" t="s">
         <v>61</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" t="s">
         <v>64</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E24" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="14">
+      <c r="F24" s="5">
         <v>45791</v>
       </c>
       <c r="G24" s="6">
@@ -1500,6 +1549,11 @@
         <v>79.989999999999995</v>
       </c>
     </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+    </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>17</v>
@@ -1527,16 +1581,16 @@
       <c r="A29" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" t="s">
         <v>32</v>
       </c>
-      <c r="E29" s="13" t="s">
+      <c r="E29" t="s">
         <v>71</v>
       </c>
       <c r="F29" s="11" t="s">
@@ -1595,8 +1649,11 @@
       <c r="E34" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="2" t="s">
         <v>22</v>
+      </c>
+      <c r="G34" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
@@ -1615,8 +1672,11 @@
       <c r="E35" s="5">
         <v>45820</v>
       </c>
-      <c r="F35" s="6">
+      <c r="F35" s="13">
         <v>19.989999999999998</v>
+      </c>
+      <c r="G35" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
@@ -1635,8 +1695,11 @@
       <c r="E36" s="5">
         <v>45836</v>
       </c>
-      <c r="F36" s="6">
+      <c r="F36" s="13">
         <v>119.98</v>
+      </c>
+      <c r="G36" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
@@ -1655,8 +1718,11 @@
       <c r="E37" s="5">
         <v>45836</v>
       </c>
-      <c r="F37" s="6">
+      <c r="F37" s="13">
         <v>119.98</v>
+      </c>
+      <c r="G37" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
@@ -1675,8 +1741,11 @@
       <c r="E38" s="9">
         <v>45841</v>
       </c>
-      <c r="F38" s="10">
+      <c r="F38" s="8">
         <v>79.989999999999995</v>
+      </c>
+      <c r="G38" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
@@ -1874,10 +1943,10 @@
       <c r="A52" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B52" s="13" t="s">
+      <c r="B52" t="s">
         <v>45</v>
       </c>
-      <c r="C52" s="13" t="s">
+      <c r="C52" t="s">
         <v>18</v>
       </c>
       <c r="D52" s="6">
@@ -1892,7 +1961,7 @@
       <c r="H52" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I52" s="18" t="s">
+      <c r="I52" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1900,10 +1969,10 @@
       <c r="A53" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B53" s="13" t="s">
+      <c r="B53" t="s">
         <v>46</v>
       </c>
-      <c r="C53" s="13" t="s">
+      <c r="C53" t="s">
         <v>18</v>
       </c>
       <c r="D53" s="6">
@@ -1912,10 +1981,10 @@
       <c r="F53" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G53" s="13" t="s">
+      <c r="G53" t="s">
         <v>56</v>
       </c>
-      <c r="H53" s="13" t="s">
+      <c r="H53" t="s">
         <v>58</v>
       </c>
       <c r="I53" s="6">
@@ -1926,10 +1995,10 @@
       <c r="A54" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B54" s="13" t="s">
+      <c r="B54" t="s">
         <v>47</v>
       </c>
-      <c r="C54" s="13" t="s">
+      <c r="C54" t="s">
         <v>19</v>
       </c>
       <c r="D54" s="6">
@@ -1949,13 +2018,13 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A55" s="16" t="s">
+      <c r="A55" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B55" s="15" t="s">
+      <c r="B55" t="s">
         <v>85</v>
       </c>
-      <c r="C55" s="13" t="s">
+      <c r="C55" t="s">
         <v>18</v>
       </c>
       <c r="D55" s="6">
@@ -1963,7 +2032,7 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A56" s="17" t="s">
+      <c r="A56" s="7" t="s">
         <v>84</v>
       </c>
       <c r="B56" s="8" t="s">

</xml_diff>